<commit_message>
Production Schedule (Pre-Production). Design focused currently, and dates may be wrong
</commit_message>
<xml_diff>
--- a/Documentation/Quantum Dynamics - Production Schedule.xlsx
+++ b/Documentation/Quantum Dynamics - Production Schedule.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s181532\Documents\QuantiumDynamics\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38298B5-2E7E-48C5-A887-5523AD99A817}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{D98885EC-5622-42FC-9DFB-2B490A2CB657}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PreProduction" sheetId="1" r:id="rId1"/>
     <sheet name="Production" sheetId="3" r:id="rId2"/>
     <sheet name="Final" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>|_ Game Design</t>
   </si>
@@ -76,12 +70,6 @@
     <t>|_ Mechanics: Time - Pause</t>
   </si>
   <si>
-    <t>|_ Mechanics: Time - Fast Forward</t>
-  </si>
-  <si>
-    <t>|_ Mechanics: Time - Rewind</t>
-  </si>
-  <si>
     <t>|_ Player Character</t>
   </si>
   <si>
@@ -92,13 +80,124 @@
   </si>
   <si>
     <t>|_ User Interface</t>
+  </si>
+  <si>
+    <t>Onwards</t>
+  </si>
+  <si>
+    <t>Narrative:</t>
+  </si>
+  <si>
+    <t>Mechanics:</t>
+  </si>
+  <si>
+    <t>Level Design:</t>
+  </si>
+  <si>
+    <t>Paper prototype</t>
+  </si>
+  <si>
+    <t>Narrative breakdown</t>
+  </si>
+  <si>
+    <t>Gravity puzzles</t>
+  </si>
+  <si>
+    <t>Time slow puzzles</t>
+  </si>
+  <si>
+    <t>Time stop puzzles</t>
+  </si>
+  <si>
+    <t>Teleportation puzzles</t>
+  </si>
+  <si>
+    <t>Hybrid puzzles</t>
+  </si>
+  <si>
+    <t>Level test implementation</t>
+  </si>
+  <si>
+    <t>Testing:</t>
+  </si>
+  <si>
+    <t>Andy backstory</t>
+  </si>
+  <si>
+    <t>Ryan (creator) backstory</t>
+  </si>
+  <si>
+    <t>Jason (evil scientist) backstory</t>
+  </si>
+  <si>
+    <t>Dialogue scripting (actual dialogue)</t>
+  </si>
+  <si>
+    <t>Narrative scripting (event based code)</t>
+  </si>
+  <si>
+    <t>Diagetic narrative planning</t>
+  </si>
+  <si>
+    <t>Tutorial creation</t>
+  </si>
+  <si>
+    <t>Interactable (doors, moving platforms, etc)</t>
+  </si>
+  <si>
+    <t>Gravity</t>
+  </si>
+  <si>
+    <t>Time slow</t>
+  </si>
+  <si>
+    <t>Time stop</t>
+  </si>
+  <si>
+    <t>Teleportation</t>
+  </si>
+  <si>
+    <t>Object selection (modularity; one selection to control all abilities)</t>
+  </si>
+  <si>
+    <t>Player gravity testing</t>
+  </si>
+  <si>
+    <t>Other/global gravity testing</t>
+  </si>
+  <si>
+    <t>Time slow testing</t>
+  </si>
+  <si>
+    <t>Time stop testing</t>
+  </si>
+  <si>
+    <t>Pick-up objects</t>
+  </si>
+  <si>
+    <t>Control mapping testing</t>
+  </si>
+  <si>
+    <t>Teleportation testing</t>
+  </si>
+  <si>
+    <t>Kleenex Tests</t>
+  </si>
+  <si>
+    <t>Tutorial testing</t>
+  </si>
+  <si>
+    <t>Narrative flow testing</t>
+  </si>
+  <si>
+    <t>Level testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,16 +213,83 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -131,46 +297,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <strike val="0"/>
@@ -499,21 +687,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56152718-2DD9-41BA-B394-2F320B84C4F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:FL23"/>
+  <dimension ref="A1:AN22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +711,7 @@
     <col min="2" max="168" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:168" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>43649</v>
       </c>
@@ -637,494 +826,438 @@
       <c r="AM1" s="2">
         <v>43686</v>
       </c>
-      <c r="AN1" s="2">
-        <v>43687</v>
-      </c>
-      <c r="AO1" s="2">
-        <v>43688</v>
-      </c>
-      <c r="AP1" s="2">
-        <v>43689</v>
-      </c>
-      <c r="AQ1" s="2">
-        <v>43690</v>
-      </c>
-      <c r="AR1" s="2">
-        <v>43691</v>
-      </c>
-      <c r="AS1" s="2">
-        <v>43692</v>
-      </c>
-      <c r="AT1" s="2">
-        <v>43693</v>
-      </c>
-      <c r="AU1" s="2">
-        <v>43694</v>
-      </c>
-      <c r="AV1" s="2">
-        <v>43695</v>
-      </c>
-      <c r="AW1" s="2">
-        <v>43696</v>
-      </c>
-      <c r="AX1" s="2">
-        <v>43697</v>
-      </c>
-      <c r="AY1" s="2">
-        <v>43698</v>
-      </c>
-      <c r="AZ1" s="2">
-        <v>43699</v>
-      </c>
-      <c r="BA1" s="2">
-        <v>43700</v>
-      </c>
-      <c r="BB1" s="2">
-        <v>43701</v>
-      </c>
-      <c r="BC1" s="2">
-        <v>43702</v>
-      </c>
-      <c r="BD1" s="2">
-        <v>43703</v>
-      </c>
-      <c r="BE1" s="2">
-        <v>43704</v>
-      </c>
-      <c r="BF1" s="2">
-        <v>43705</v>
-      </c>
-      <c r="BG1" s="2">
-        <v>43706</v>
-      </c>
-      <c r="BH1" s="2">
-        <v>43707</v>
-      </c>
-      <c r="BI1" s="2">
-        <v>43708</v>
-      </c>
-      <c r="BJ1" s="2">
-        <v>43709</v>
-      </c>
-      <c r="BK1" s="2">
-        <v>43710</v>
-      </c>
-      <c r="BL1" s="2">
-        <v>43711</v>
-      </c>
-      <c r="BM1" s="2">
-        <v>43712</v>
-      </c>
-      <c r="BN1" s="2">
-        <v>43713</v>
-      </c>
-      <c r="BO1" s="2">
-        <v>43714</v>
-      </c>
-      <c r="BP1" s="2">
-        <v>43715</v>
-      </c>
-      <c r="BQ1" s="2">
-        <v>43716</v>
-      </c>
-      <c r="BR1" s="2">
-        <v>43717</v>
-      </c>
-      <c r="BS1" s="2">
-        <v>43718</v>
-      </c>
-      <c r="BT1" s="2">
-        <v>43719</v>
-      </c>
-      <c r="BU1" s="2">
-        <v>43720</v>
-      </c>
-      <c r="BV1" s="2">
-        <v>43721</v>
-      </c>
-      <c r="BW1" s="2">
-        <v>43722</v>
-      </c>
-      <c r="BX1" s="2">
-        <v>43723</v>
-      </c>
-      <c r="BY1" s="2">
-        <v>43724</v>
-      </c>
-      <c r="BZ1" s="2">
-        <v>43725</v>
-      </c>
-      <c r="CA1" s="2">
-        <v>43726</v>
-      </c>
-      <c r="CB1" s="2">
-        <v>43727</v>
-      </c>
-      <c r="CC1" s="2">
-        <v>43728</v>
-      </c>
-      <c r="CD1" s="2">
-        <v>43729</v>
-      </c>
-      <c r="CE1" s="2">
-        <v>43730</v>
-      </c>
-      <c r="CF1" s="2">
-        <v>43731</v>
-      </c>
-      <c r="CG1" s="2">
-        <v>43732</v>
-      </c>
-      <c r="CH1" s="2">
-        <v>43733</v>
-      </c>
-      <c r="CI1" s="2">
-        <v>43734</v>
-      </c>
-      <c r="CJ1" s="2">
-        <v>43735</v>
-      </c>
-      <c r="CK1" s="2">
-        <v>43736</v>
-      </c>
-      <c r="CL1" s="2">
-        <v>43737</v>
-      </c>
-      <c r="CM1" s="2">
-        <v>43738</v>
-      </c>
-      <c r="CN1" s="2">
-        <v>43739</v>
-      </c>
-      <c r="CO1" s="2">
-        <v>43740</v>
-      </c>
-      <c r="CP1" s="2">
-        <v>43741</v>
-      </c>
-      <c r="CQ1" s="2">
-        <v>43742</v>
-      </c>
-      <c r="CR1" s="2">
-        <v>43743</v>
-      </c>
-      <c r="CS1" s="2">
-        <v>43744</v>
-      </c>
-      <c r="CT1" s="2">
-        <v>43745</v>
-      </c>
-      <c r="CU1" s="2">
-        <v>43746</v>
-      </c>
-      <c r="CV1" s="2">
-        <v>43747</v>
-      </c>
-      <c r="CW1" s="2">
-        <v>43748</v>
-      </c>
-      <c r="CX1" s="2">
-        <v>43749</v>
-      </c>
-      <c r="CY1" s="2">
-        <v>43750</v>
-      </c>
-      <c r="CZ1" s="2">
-        <v>43751</v>
-      </c>
-      <c r="DA1" s="2">
-        <v>43752</v>
-      </c>
-      <c r="DB1" s="2">
-        <v>43753</v>
-      </c>
-      <c r="DC1" s="2">
-        <v>43754</v>
-      </c>
-      <c r="DD1" s="2">
-        <v>43755</v>
-      </c>
-      <c r="DE1" s="2">
-        <v>43756</v>
-      </c>
-      <c r="DF1" s="2">
-        <v>43757</v>
-      </c>
-      <c r="DG1" s="2">
-        <v>43758</v>
-      </c>
-      <c r="DH1" s="2">
-        <v>43759</v>
-      </c>
-      <c r="DI1" s="2">
-        <v>43760</v>
-      </c>
-      <c r="DJ1" s="2">
-        <v>43761</v>
-      </c>
-      <c r="DK1" s="2">
-        <v>43762</v>
-      </c>
-      <c r="DL1" s="2">
-        <v>43763</v>
-      </c>
-      <c r="DM1" s="2">
-        <v>43764</v>
-      </c>
-      <c r="DN1" s="2">
-        <v>43765</v>
-      </c>
-      <c r="DO1" s="2">
-        <v>43766</v>
-      </c>
-      <c r="DP1" s="2">
-        <v>43767</v>
-      </c>
-      <c r="DQ1" s="2">
-        <v>43768</v>
-      </c>
-      <c r="DR1" s="2">
-        <v>43769</v>
-      </c>
-      <c r="DS1" s="2">
-        <v>43770</v>
-      </c>
-      <c r="DT1" s="2">
-        <v>43771</v>
-      </c>
-      <c r="DU1" s="2">
-        <v>43772</v>
-      </c>
-      <c r="DV1" s="2">
-        <v>43773</v>
-      </c>
-      <c r="DW1" s="2">
-        <v>43774</v>
-      </c>
-      <c r="DX1" s="2">
-        <v>43775</v>
-      </c>
-      <c r="DY1" s="2">
-        <v>43776</v>
-      </c>
-      <c r="DZ1" s="2">
-        <v>43777</v>
-      </c>
-      <c r="EA1" s="2">
-        <v>43778</v>
-      </c>
-      <c r="EB1" s="2">
-        <v>43779</v>
-      </c>
-      <c r="EC1" s="2">
-        <v>43780</v>
-      </c>
-      <c r="ED1" s="2">
-        <v>43781</v>
-      </c>
-      <c r="EE1" s="2">
-        <v>43782</v>
-      </c>
-      <c r="EF1" s="2">
-        <v>43783</v>
-      </c>
-      <c r="EG1" s="2">
-        <v>43784</v>
-      </c>
-      <c r="EH1" s="2">
-        <v>43785</v>
-      </c>
-      <c r="EI1" s="2">
-        <v>43786</v>
-      </c>
-      <c r="EJ1" s="2">
-        <v>43787</v>
-      </c>
-      <c r="EK1" s="2">
-        <v>43788</v>
-      </c>
-      <c r="EL1" s="2">
-        <v>43789</v>
-      </c>
-      <c r="EM1" s="2">
-        <v>43790</v>
-      </c>
-      <c r="EN1" s="2">
-        <v>43791</v>
-      </c>
-      <c r="EO1" s="2">
-        <v>43792</v>
-      </c>
-      <c r="EP1" s="2">
-        <v>43793</v>
-      </c>
-      <c r="EQ1" s="2">
-        <v>43794</v>
-      </c>
-      <c r="ER1" s="2">
-        <v>43795</v>
-      </c>
-      <c r="ES1" s="2">
-        <v>43796</v>
-      </c>
-      <c r="ET1" s="2">
-        <v>43797</v>
-      </c>
-      <c r="EU1" s="2">
-        <v>43798</v>
-      </c>
-      <c r="EV1" s="2">
-        <v>43799</v>
-      </c>
-      <c r="EW1" s="2">
-        <v>43800</v>
-      </c>
-      <c r="EX1" s="2">
-        <v>43801</v>
-      </c>
-      <c r="EY1" s="2">
-        <v>43802</v>
-      </c>
-      <c r="EZ1" s="2">
-        <v>43803</v>
-      </c>
-      <c r="FA1" s="2">
-        <v>43804</v>
-      </c>
-      <c r="FB1" s="2">
-        <v>43805</v>
-      </c>
-      <c r="FC1" s="2">
-        <v>43806</v>
-      </c>
-      <c r="FD1" s="2">
-        <v>43807</v>
-      </c>
-      <c r="FE1" s="2">
-        <v>43808</v>
-      </c>
-      <c r="FF1" s="2">
-        <v>43809</v>
-      </c>
-      <c r="FG1" s="2">
-        <v>43810</v>
-      </c>
-      <c r="FH1" s="2">
-        <v>43811</v>
-      </c>
-      <c r="FI1" s="2">
-        <v>43812</v>
-      </c>
-      <c r="FJ1" s="2">
-        <v>43813</v>
-      </c>
-      <c r="FK1" s="2">
-        <v>43814</v>
-      </c>
-      <c r="FL1" s="2">
-        <v>43815</v>
-      </c>
-    </row>
-    <row r="2" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="AN1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:168" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:168" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:168" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:168" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:168" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:168" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+    </row>
+    <row r="19" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="20" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8"/>
+    </row>
+    <row r="21" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
-    </row>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8"/>
+    </row>
+    <row r="22" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="B2">
     <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today">
@@ -1137,531 +1270,608 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECACF59-3304-4DFB-BFD0-615643426CF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:FL1"/>
+  <dimension ref="A1:EA41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="168" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:168" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:131" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
-        <v>43649</v>
+        <v>43686</v>
       </c>
       <c r="C1" s="1">
-        <v>43650</v>
+        <v>43687</v>
       </c>
       <c r="D1" s="1">
-        <v>43651</v>
+        <v>43688</v>
       </c>
       <c r="E1" s="1">
-        <v>43652</v>
+        <v>43689</v>
       </c>
       <c r="F1" s="1">
-        <v>43653</v>
+        <v>43690</v>
       </c>
       <c r="G1" s="1">
-        <v>43654</v>
+        <v>43691</v>
       </c>
       <c r="H1" s="1">
-        <v>43655</v>
+        <v>43692</v>
       </c>
       <c r="I1" s="1">
-        <v>43656</v>
+        <v>43693</v>
       </c>
       <c r="J1" s="1">
-        <v>43657</v>
+        <v>43694</v>
       </c>
       <c r="K1" s="1">
-        <v>43658</v>
+        <v>43695</v>
       </c>
       <c r="L1" s="1">
-        <v>43659</v>
+        <v>43696</v>
       </c>
       <c r="M1" s="1">
-        <v>43660</v>
+        <v>43697</v>
       </c>
       <c r="N1" s="1">
-        <v>43661</v>
+        <v>43698</v>
       </c>
       <c r="O1" s="1">
-        <v>43662</v>
+        <v>43699</v>
       </c>
       <c r="P1" s="1">
-        <v>43663</v>
+        <v>43700</v>
       </c>
       <c r="Q1" s="1">
-        <v>43664</v>
+        <v>43701</v>
       </c>
       <c r="R1" s="1">
-        <v>43665</v>
+        <v>43702</v>
       </c>
       <c r="S1" s="1">
-        <v>43666</v>
+        <v>43703</v>
       </c>
       <c r="T1" s="1">
-        <v>43667</v>
+        <v>43704</v>
       </c>
       <c r="U1" s="1">
-        <v>43668</v>
+        <v>43705</v>
       </c>
       <c r="V1" s="1">
-        <v>43669</v>
+        <v>43706</v>
       </c>
       <c r="W1" s="1">
-        <v>43670</v>
+        <v>43707</v>
       </c>
       <c r="X1" s="1">
-        <v>43671</v>
+        <v>43708</v>
       </c>
       <c r="Y1" s="1">
-        <v>43672</v>
+        <v>43709</v>
       </c>
       <c r="Z1" s="1">
-        <v>43673</v>
+        <v>43710</v>
       </c>
       <c r="AA1" s="1">
-        <v>43674</v>
+        <v>43711</v>
       </c>
       <c r="AB1" s="1">
-        <v>43675</v>
+        <v>43712</v>
       </c>
       <c r="AC1" s="1">
-        <v>43676</v>
+        <v>43713</v>
       </c>
       <c r="AD1" s="1">
-        <v>43677</v>
+        <v>43714</v>
       </c>
       <c r="AE1" s="1">
-        <v>43678</v>
+        <v>43715</v>
       </c>
       <c r="AF1" s="1">
-        <v>43679</v>
+        <v>43716</v>
       </c>
       <c r="AG1" s="1">
-        <v>43680</v>
+        <v>43717</v>
       </c>
       <c r="AH1" s="1">
-        <v>43681</v>
+        <v>43718</v>
       </c>
       <c r="AI1" s="1">
-        <v>43682</v>
+        <v>43719</v>
       </c>
       <c r="AJ1" s="1">
-        <v>43683</v>
+        <v>43720</v>
       </c>
       <c r="AK1" s="1">
-        <v>43684</v>
+        <v>43721</v>
       </c>
       <c r="AL1" s="1">
-        <v>43685</v>
+        <v>43722</v>
       </c>
       <c r="AM1" s="1">
-        <v>43686</v>
+        <v>43723</v>
       </c>
       <c r="AN1" s="1">
-        <v>43687</v>
+        <v>43724</v>
       </c>
       <c r="AO1" s="1">
-        <v>43688</v>
+        <v>43725</v>
       </c>
       <c r="AP1" s="1">
-        <v>43689</v>
+        <v>43726</v>
       </c>
       <c r="AQ1" s="1">
-        <v>43690</v>
+        <v>43727</v>
       </c>
       <c r="AR1" s="1">
-        <v>43691</v>
+        <v>43728</v>
       </c>
       <c r="AS1" s="1">
-        <v>43692</v>
+        <v>43729</v>
       </c>
       <c r="AT1" s="1">
-        <v>43693</v>
+        <v>43730</v>
       </c>
       <c r="AU1" s="1">
-        <v>43694</v>
+        <v>43731</v>
       </c>
       <c r="AV1" s="1">
-        <v>43695</v>
+        <v>43732</v>
       </c>
       <c r="AW1" s="1">
-        <v>43696</v>
+        <v>43733</v>
       </c>
       <c r="AX1" s="1">
-        <v>43697</v>
+        <v>43734</v>
       </c>
       <c r="AY1" s="1">
-        <v>43698</v>
+        <v>43735</v>
       </c>
       <c r="AZ1" s="1">
-        <v>43699</v>
+        <v>43736</v>
       </c>
       <c r="BA1" s="1">
-        <v>43700</v>
+        <v>43737</v>
       </c>
       <c r="BB1" s="1">
-        <v>43701</v>
+        <v>43738</v>
       </c>
       <c r="BC1" s="1">
-        <v>43702</v>
+        <v>43739</v>
       </c>
       <c r="BD1" s="1">
-        <v>43703</v>
+        <v>43740</v>
       </c>
       <c r="BE1" s="1">
-        <v>43704</v>
+        <v>43741</v>
       </c>
       <c r="BF1" s="1">
-        <v>43705</v>
+        <v>43742</v>
       </c>
       <c r="BG1" s="1">
-        <v>43706</v>
+        <v>43743</v>
       </c>
       <c r="BH1" s="1">
-        <v>43707</v>
+        <v>43744</v>
       </c>
       <c r="BI1" s="1">
-        <v>43708</v>
+        <v>43745</v>
       </c>
       <c r="BJ1" s="1">
-        <v>43709</v>
+        <v>43746</v>
       </c>
       <c r="BK1" s="1">
-        <v>43710</v>
+        <v>43747</v>
       </c>
       <c r="BL1" s="1">
-        <v>43711</v>
+        <v>43748</v>
       </c>
       <c r="BM1" s="1">
-        <v>43712</v>
+        <v>43749</v>
       </c>
       <c r="BN1" s="1">
-        <v>43713</v>
+        <v>43750</v>
       </c>
       <c r="BO1" s="1">
-        <v>43714</v>
+        <v>43751</v>
       </c>
       <c r="BP1" s="1">
-        <v>43715</v>
+        <v>43752</v>
       </c>
       <c r="BQ1" s="1">
-        <v>43716</v>
+        <v>43753</v>
       </c>
       <c r="BR1" s="1">
-        <v>43717</v>
+        <v>43754</v>
       </c>
       <c r="BS1" s="1">
-        <v>43718</v>
+        <v>43755</v>
       </c>
       <c r="BT1" s="1">
-        <v>43719</v>
+        <v>43756</v>
       </c>
       <c r="BU1" s="1">
-        <v>43720</v>
+        <v>43757</v>
       </c>
       <c r="BV1" s="1">
-        <v>43721</v>
+        <v>43758</v>
       </c>
       <c r="BW1" s="1">
-        <v>43722</v>
+        <v>43759</v>
       </c>
       <c r="BX1" s="1">
-        <v>43723</v>
+        <v>43760</v>
       </c>
       <c r="BY1" s="1">
-        <v>43724</v>
+        <v>43761</v>
       </c>
       <c r="BZ1" s="1">
-        <v>43725</v>
+        <v>43762</v>
       </c>
       <c r="CA1" s="1">
-        <v>43726</v>
+        <v>43763</v>
       </c>
       <c r="CB1" s="1">
-        <v>43727</v>
+        <v>43764</v>
       </c>
       <c r="CC1" s="1">
-        <v>43728</v>
+        <v>43765</v>
       </c>
       <c r="CD1" s="1">
-        <v>43729</v>
+        <v>43766</v>
       </c>
       <c r="CE1" s="1">
-        <v>43730</v>
+        <v>43767</v>
       </c>
       <c r="CF1" s="1">
-        <v>43731</v>
+        <v>43768</v>
       </c>
       <c r="CG1" s="1">
-        <v>43732</v>
+        <v>43769</v>
       </c>
       <c r="CH1" s="1">
-        <v>43733</v>
+        <v>43770</v>
       </c>
       <c r="CI1" s="1">
-        <v>43734</v>
+        <v>43771</v>
       </c>
       <c r="CJ1" s="1">
-        <v>43735</v>
+        <v>43772</v>
       </c>
       <c r="CK1" s="1">
-        <v>43736</v>
+        <v>43773</v>
       </c>
       <c r="CL1" s="1">
-        <v>43737</v>
+        <v>43774</v>
       </c>
       <c r="CM1" s="1">
-        <v>43738</v>
+        <v>43775</v>
       </c>
       <c r="CN1" s="1">
-        <v>43739</v>
+        <v>43776</v>
       </c>
       <c r="CO1" s="1">
-        <v>43740</v>
+        <v>43777</v>
       </c>
       <c r="CP1" s="1">
-        <v>43741</v>
+        <v>43778</v>
       </c>
       <c r="CQ1" s="1">
-        <v>43742</v>
+        <v>43779</v>
       </c>
       <c r="CR1" s="1">
-        <v>43743</v>
+        <v>43780</v>
       </c>
       <c r="CS1" s="1">
-        <v>43744</v>
+        <v>43781</v>
       </c>
       <c r="CT1" s="1">
-        <v>43745</v>
+        <v>43782</v>
       </c>
       <c r="CU1" s="1">
-        <v>43746</v>
+        <v>43783</v>
       </c>
       <c r="CV1" s="1">
-        <v>43747</v>
+        <v>43784</v>
       </c>
       <c r="CW1" s="1">
-        <v>43748</v>
+        <v>43785</v>
       </c>
       <c r="CX1" s="1">
-        <v>43749</v>
+        <v>43786</v>
       </c>
       <c r="CY1" s="1">
-        <v>43750</v>
+        <v>43787</v>
       </c>
       <c r="CZ1" s="1">
-        <v>43751</v>
+        <v>43788</v>
       </c>
       <c r="DA1" s="1">
-        <v>43752</v>
+        <v>43789</v>
       </c>
       <c r="DB1" s="1">
-        <v>43753</v>
+        <v>43790</v>
       </c>
       <c r="DC1" s="1">
-        <v>43754</v>
+        <v>43791</v>
       </c>
       <c r="DD1" s="1">
-        <v>43755</v>
+        <v>43792</v>
       </c>
       <c r="DE1" s="1">
-        <v>43756</v>
+        <v>43793</v>
       </c>
       <c r="DF1" s="1">
-        <v>43757</v>
+        <v>43794</v>
       </c>
       <c r="DG1" s="1">
-        <v>43758</v>
+        <v>43795</v>
       </c>
       <c r="DH1" s="1">
-        <v>43759</v>
+        <v>43796</v>
       </c>
       <c r="DI1" s="1">
-        <v>43760</v>
+        <v>43797</v>
       </c>
       <c r="DJ1" s="1">
-        <v>43761</v>
+        <v>43798</v>
       </c>
       <c r="DK1" s="1">
-        <v>43762</v>
+        <v>43799</v>
       </c>
       <c r="DL1" s="1">
-        <v>43763</v>
+        <v>43800</v>
       </c>
       <c r="DM1" s="1">
-        <v>43764</v>
+        <v>43801</v>
       </c>
       <c r="DN1" s="1">
-        <v>43765</v>
+        <v>43802</v>
       </c>
       <c r="DO1" s="1">
-        <v>43766</v>
+        <v>43803</v>
       </c>
       <c r="DP1" s="1">
-        <v>43767</v>
+        <v>43804</v>
       </c>
       <c r="DQ1" s="1">
-        <v>43768</v>
+        <v>43805</v>
       </c>
       <c r="DR1" s="1">
-        <v>43769</v>
+        <v>43806</v>
       </c>
       <c r="DS1" s="1">
-        <v>43770</v>
+        <v>43807</v>
       </c>
       <c r="DT1" s="1">
-        <v>43771</v>
+        <v>43808</v>
       </c>
       <c r="DU1" s="1">
-        <v>43772</v>
+        <v>43809</v>
       </c>
       <c r="DV1" s="1">
-        <v>43773</v>
+        <v>43810</v>
       </c>
       <c r="DW1" s="1">
-        <v>43774</v>
+        <v>43811</v>
       </c>
       <c r="DX1" s="1">
-        <v>43775</v>
+        <v>43812</v>
       </c>
       <c r="DY1" s="1">
-        <v>43776</v>
+        <v>43813</v>
       </c>
       <c r="DZ1" s="1">
-        <v>43777</v>
+        <v>43814</v>
       </c>
       <c r="EA1" s="1">
-        <v>43778</v>
-      </c>
-      <c r="EB1" s="1">
-        <v>43779</v>
-      </c>
-      <c r="EC1" s="1">
-        <v>43780</v>
-      </c>
-      <c r="ED1" s="1">
-        <v>43781</v>
-      </c>
-      <c r="EE1" s="1">
-        <v>43782</v>
-      </c>
-      <c r="EF1" s="1">
-        <v>43783</v>
-      </c>
-      <c r="EG1" s="1">
-        <v>43784</v>
-      </c>
-      <c r="EH1" s="1">
-        <v>43785</v>
-      </c>
-      <c r="EI1" s="1">
-        <v>43786</v>
-      </c>
-      <c r="EJ1" s="1">
-        <v>43787</v>
-      </c>
-      <c r="EK1" s="1">
-        <v>43788</v>
-      </c>
-      <c r="EL1" s="1">
-        <v>43789</v>
-      </c>
-      <c r="EM1" s="1">
-        <v>43790</v>
-      </c>
-      <c r="EN1" s="1">
-        <v>43791</v>
-      </c>
-      <c r="EO1" s="1">
-        <v>43792</v>
-      </c>
-      <c r="EP1" s="1">
-        <v>43793</v>
-      </c>
-      <c r="EQ1" s="1">
-        <v>43794</v>
-      </c>
-      <c r="ER1" s="1">
-        <v>43795</v>
-      </c>
-      <c r="ES1" s="1">
-        <v>43796</v>
-      </c>
-      <c r="ET1" s="1">
-        <v>43797</v>
-      </c>
-      <c r="EU1" s="1">
-        <v>43798</v>
-      </c>
-      <c r="EV1" s="1">
-        <v>43799</v>
-      </c>
-      <c r="EW1" s="1">
-        <v>43800</v>
-      </c>
-      <c r="EX1" s="1">
-        <v>43801</v>
-      </c>
-      <c r="EY1" s="1">
-        <v>43802</v>
-      </c>
-      <c r="EZ1" s="1">
-        <v>43803</v>
-      </c>
-      <c r="FA1" s="1">
-        <v>43804</v>
-      </c>
-      <c r="FB1" s="1">
-        <v>43805</v>
-      </c>
-      <c r="FC1" s="1">
-        <v>43806</v>
-      </c>
-      <c r="FD1" s="1">
-        <v>43807</v>
-      </c>
-      <c r="FE1" s="1">
-        <v>43808</v>
-      </c>
-      <c r="FF1" s="1">
-        <v>43809</v>
-      </c>
-      <c r="FG1" s="1">
-        <v>43810</v>
-      </c>
-      <c r="FH1" s="1">
-        <v>43811</v>
-      </c>
-      <c r="FI1" s="1">
-        <v>43812</v>
-      </c>
-      <c r="FJ1" s="1">
-        <v>43813</v>
-      </c>
-      <c r="FK1" s="1">
-        <v>43814</v>
-      </c>
-      <c r="FL1" s="1">
         <v>43815</v>
+      </c>
+    </row>
+    <row r="2" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:131" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252673BE-7511-4E2E-BBDC-E3CF29298F7A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>

</xml_diff>